<commit_message>
Farsi excel updated and spaces removed from file names
	- farsi excel udpated with all words from Punjabi farsi pdf
	- spaces removed from filenames
</commit_message>
<xml_diff>
--- a/Farsi/farsi.xlsx
+++ b/Farsi/farsi.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qualcomm-my.sharepoint.com/personal/tajinder_qti_qualcomm_com/Documents/Documents/Backup/farsi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tajinder\OneDrive - Qualcomm\Documents\GitHub\daraaj\Farsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="374" documentId="8_{FEDFE9AF-6B4A-47FD-BE71-62D6574CB582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56188F1B-7D86-4CEC-B133-83C28AE18A3F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11BBFA39-6659-4052-A245-483E1B2789FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AAE7113E-29B1-41C8-96BE-EEA64320B172}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AAE7113E-29B1-41C8-96BE-EEA64320B172}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="323">
   <si>
     <t>معانی</t>
   </si>
@@ -737,6 +738,273 @@
   </si>
   <si>
     <t>ਅਰਾਮ ਕਰ</t>
+  </si>
+  <si>
+    <t>ਛਿੱਲਣਾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਕੱਟਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਛੁਟਕਾਰਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਜੀਊਣ </t>
+  </si>
+  <si>
+    <t>ਗਾਣਾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਤੋੜਨਾ ਟੁਟਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਲਿਬੜਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਉਭਾਰਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਪਰਤਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸੁੰਘਣਾਂ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸਵਿਕਾਰ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਨਾਪਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਛਿੱਲਣਾ </t>
+  </si>
+  <si>
+    <t>ਚਰਨਾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚਮਕਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਲੜਾਈ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਕਰਨੀ </t>
+  </si>
+  <si>
+    <t>ਚੀਰਨਾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਪਾੜਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਬੁਲਾਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਊਂਘਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਘਿਸਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਕੁੱਟਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਪਿਘਲਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਛੱਡਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਵੱਢਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸਮਾਉਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਕੰਬਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਮਲਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਨਾਜ਼ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਦੇਖਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਕਿਰਪਾ ਕਰਨੀ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਡਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚਲਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਆਰਾਮ ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਅਰੰਭ ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸੁੱਟਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਜਾਲਣਾ </t>
+  </si>
+  <si>
+    <t>ਬੁੱਝਣਾ</t>
+  </si>
+  <si>
+    <t>ਉੱਚਾ ਕਰਨਾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਪੂਜਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸੰਵਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਟਪਕਣਾ ਰਿਸਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਹਿੱਲਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚੱਖਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਟਪਕਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਉੱਠਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸ਼ੋਰ ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚੁੱਪ ਰਹਿਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸੋਂਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਫੂਕਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚੋਣਾਂ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਲੈ ਭੱਜਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਕੱਤਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਨੱਚਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਝਾੜੂ ਦੇਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਭੱਜਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਜੰਮਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚੰਗਾ ਲੱਗਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸਪੁਰਦ ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਤੋਲਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਲਾਇਕ ਹੋਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸਬਰ ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਦੌੜਨਾ ਛੇਤੀ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਤਪਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਮੋਹਿਤ ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਵਧਾਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਘਟਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਖੋਦਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਮਾਇਲ  ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t>ਫਿਰਨਾ</t>
+  </si>
+  <si>
+    <t>ਬਿਛਾਣਾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਗੱਪ ਮਾਰਨੀ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਢੂੰਢਣਾ </t>
+  </si>
+  <si>
+    <t>ਲਪੇਟਣਾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਤਿੜਕਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚੰਬੜਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਚੁਭਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਝੁਕੱਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਹੱਕਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਸੋਚਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਗ਼ਮ ਖਾਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਹਜ਼ਮ ਹੋਂਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਨਿਚੋੜ ਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਭੁੰਨਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਰੁਝਣਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਖਾਲੀ ਕਰਨਾ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ਲਬੇੜਨਾ </t>
   </si>
 </sst>
 </file>
@@ -758,7 +1026,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -786,6 +1054,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,7 +1170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -927,6 +1207,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,9 +1237,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -985,7 +1277,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1091,7 +1383,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1233,7 +1525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1242,10 +1534,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4253A2-C708-4B3E-B4F5-74A924887BCB}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A3:U103"/>
+  <dimension ref="A3:U200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C71" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D197" sqref="D197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3081,6 +3373,1461 @@
       <c r="G103" s="17"/>
       <c r="H103" s="17"/>
       <c r="I103" s="17"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>100</v>
+      </c>
+      <c r="B104" s="18"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="F104" s="18"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="19"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>101</v>
+      </c>
+      <c r="B105" s="18"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="F105" s="18"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="19"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>102</v>
+      </c>
+      <c r="B106" s="18"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="F106" s="18"/>
+      <c r="G106" s="19"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="19"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>103</v>
+      </c>
+      <c r="B107" s="18"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F107" s="18"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="18"/>
+      <c r="I107" s="19"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>104</v>
+      </c>
+      <c r="B108" s="18"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="F108" s="18"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="18"/>
+      <c r="I108" s="19"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>105</v>
+      </c>
+      <c r="B109" s="18"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="F109" s="18"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="18"/>
+      <c r="I109" s="19"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>106</v>
+      </c>
+      <c r="B110" s="18"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="F110" s="18"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="19"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>107</v>
+      </c>
+      <c r="B111" s="18"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="F111" s="18"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="18"/>
+      <c r="I111" s="19"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>108</v>
+      </c>
+      <c r="B112" s="18"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="F112" s="18"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="18"/>
+      <c r="I112" s="19"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>109</v>
+      </c>
+      <c r="B113" s="18"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="F113" s="18"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="18"/>
+      <c r="I113" s="19"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>110</v>
+      </c>
+      <c r="B114" s="18"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="F114" s="18"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="19"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>111</v>
+      </c>
+      <c r="B115" s="18"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="F115" s="18"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="18"/>
+      <c r="I115" s="19"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>112</v>
+      </c>
+      <c r="B116" s="18"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="F116" s="18"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="18"/>
+      <c r="I116" s="19"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>113</v>
+      </c>
+      <c r="B117" s="18"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="F117" s="18"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="18"/>
+      <c r="I117" s="19"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>114</v>
+      </c>
+      <c r="B118" s="18"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="F118" s="18"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="18"/>
+      <c r="I118" s="19"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>115</v>
+      </c>
+      <c r="B119" s="18"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="18"/>
+      <c r="E119" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="F119" s="18"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="18"/>
+      <c r="I119" s="19"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>116</v>
+      </c>
+      <c r="B120" s="18"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="F120" s="18"/>
+      <c r="G120" s="19"/>
+      <c r="H120" s="18"/>
+      <c r="I120" s="19"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>117</v>
+      </c>
+      <c r="B121" s="18"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="18"/>
+      <c r="E121" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="F121" s="18"/>
+      <c r="G121" s="19"/>
+      <c r="H121" s="18"/>
+      <c r="I121" s="19"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>118</v>
+      </c>
+      <c r="B122" s="18"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="F122" s="18"/>
+      <c r="G122" s="19"/>
+      <c r="H122" s="18"/>
+      <c r="I122" s="19"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>119</v>
+      </c>
+      <c r="B123" s="18"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="18"/>
+      <c r="E123" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="F123" s="18"/>
+      <c r="G123" s="19"/>
+      <c r="H123" s="18"/>
+      <c r="I123" s="19"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>120</v>
+      </c>
+      <c r="B124" s="18"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="18"/>
+      <c r="E124" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F124" s="18"/>
+      <c r="G124" s="19"/>
+      <c r="H124" s="18"/>
+      <c r="I124" s="19"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>121</v>
+      </c>
+      <c r="B125" s="20"/>
+      <c r="C125" s="21"/>
+      <c r="D125" s="20"/>
+      <c r="E125" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="F125" s="20"/>
+      <c r="G125" s="21"/>
+      <c r="H125" s="20"/>
+      <c r="I125" s="21"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>122</v>
+      </c>
+      <c r="B126" s="20"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="20"/>
+      <c r="E126" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="F126" s="20"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="20"/>
+      <c r="I126" s="21"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>123</v>
+      </c>
+      <c r="B127" s="20"/>
+      <c r="C127" s="21"/>
+      <c r="D127" s="20"/>
+      <c r="E127" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="F127" s="20"/>
+      <c r="G127" s="21"/>
+      <c r="H127" s="20"/>
+      <c r="I127" s="21"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>124</v>
+      </c>
+      <c r="B128" s="20"/>
+      <c r="C128" s="21"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="F128" s="20"/>
+      <c r="G128" s="21"/>
+      <c r="H128" s="20"/>
+      <c r="I128" s="21"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>125</v>
+      </c>
+      <c r="B129" s="20"/>
+      <c r="C129" s="21"/>
+      <c r="D129" s="20"/>
+      <c r="E129" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="F129" s="20"/>
+      <c r="G129" s="21"/>
+      <c r="H129" s="20"/>
+      <c r="I129" s="21"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>126</v>
+      </c>
+      <c r="B130" s="20"/>
+      <c r="C130" s="21"/>
+      <c r="D130" s="20"/>
+      <c r="E130" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="F130" s="20"/>
+      <c r="G130" s="21"/>
+      <c r="H130" s="20"/>
+      <c r="I130" s="21"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>127</v>
+      </c>
+      <c r="B131" s="20"/>
+      <c r="C131" s="21"/>
+      <c r="D131" s="20"/>
+      <c r="E131" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="F131" s="20"/>
+      <c r="G131" s="21"/>
+      <c r="H131" s="20"/>
+      <c r="I131" s="21"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>128</v>
+      </c>
+      <c r="B132" s="20"/>
+      <c r="C132" s="21"/>
+      <c r="D132" s="20"/>
+      <c r="E132" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F132" s="20"/>
+      <c r="G132" s="21"/>
+      <c r="H132" s="20"/>
+      <c r="I132" s="21"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>129</v>
+      </c>
+      <c r="B133" s="20"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="20"/>
+      <c r="E133" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="F133" s="20"/>
+      <c r="G133" s="21"/>
+      <c r="H133" s="20"/>
+      <c r="I133" s="21"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>130</v>
+      </c>
+      <c r="B134" s="20"/>
+      <c r="C134" s="21"/>
+      <c r="D134" s="20"/>
+      <c r="E134" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="F134" s="20"/>
+      <c r="G134" s="21"/>
+      <c r="H134" s="20"/>
+      <c r="I134" s="21"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>131</v>
+      </c>
+      <c r="B135" s="20"/>
+      <c r="C135" s="21"/>
+      <c r="D135" s="20"/>
+      <c r="E135" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="F135" s="20"/>
+      <c r="G135" s="21"/>
+      <c r="H135" s="20"/>
+      <c r="I135" s="21"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>132</v>
+      </c>
+      <c r="B136" s="20"/>
+      <c r="C136" s="21"/>
+      <c r="D136" s="20"/>
+      <c r="E136" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="F136" s="20"/>
+      <c r="G136" s="21"/>
+      <c r="H136" s="20"/>
+      <c r="I136" s="21"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>133</v>
+      </c>
+      <c r="B137" s="20"/>
+      <c r="C137" s="21"/>
+      <c r="D137" s="20"/>
+      <c r="E137" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="F137" s="20"/>
+      <c r="G137" s="21"/>
+      <c r="H137" s="20"/>
+      <c r="I137" s="21"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>134</v>
+      </c>
+      <c r="B138" s="20"/>
+      <c r="C138" s="21"/>
+      <c r="D138" s="20"/>
+      <c r="E138" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F138" s="20"/>
+      <c r="G138" s="21"/>
+      <c r="H138" s="20"/>
+      <c r="I138" s="21"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>135</v>
+      </c>
+      <c r="B139" s="20"/>
+      <c r="C139" s="21"/>
+      <c r="D139" s="20"/>
+      <c r="E139" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="F139" s="20"/>
+      <c r="G139" s="21"/>
+      <c r="H139" s="20"/>
+      <c r="I139" s="21"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>136</v>
+      </c>
+      <c r="B140" s="20"/>
+      <c r="C140" s="21"/>
+      <c r="D140" s="20"/>
+      <c r="E140" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="F140" s="20"/>
+      <c r="G140" s="21"/>
+      <c r="H140" s="20"/>
+      <c r="I140" s="21"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>137</v>
+      </c>
+      <c r="B141" s="20"/>
+      <c r="C141" s="21"/>
+      <c r="D141" s="20"/>
+      <c r="E141" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="F141" s="20"/>
+      <c r="G141" s="21"/>
+      <c r="H141" s="20"/>
+      <c r="I141" s="21"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>138</v>
+      </c>
+      <c r="B142" s="20"/>
+      <c r="C142" s="21"/>
+      <c r="D142" s="20"/>
+      <c r="E142" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="F142" s="20"/>
+      <c r="G142" s="21"/>
+      <c r="H142" s="20"/>
+      <c r="I142" s="21"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>139</v>
+      </c>
+      <c r="B143" s="20"/>
+      <c r="C143" s="21"/>
+      <c r="D143" s="20"/>
+      <c r="E143" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="F143" s="20"/>
+      <c r="G143" s="21"/>
+      <c r="H143" s="20"/>
+      <c r="I143" s="21"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>140</v>
+      </c>
+      <c r="B144" s="20"/>
+      <c r="C144" s="21"/>
+      <c r="D144" s="20"/>
+      <c r="E144" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="F144" s="20"/>
+      <c r="G144" s="21"/>
+      <c r="H144" s="20"/>
+      <c r="I144" s="21"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>141</v>
+      </c>
+      <c r="B145" s="22"/>
+      <c r="C145" s="23"/>
+      <c r="D145" s="22"/>
+      <c r="E145" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="F145" s="22"/>
+      <c r="G145" s="23"/>
+      <c r="H145" s="22"/>
+      <c r="I145" s="23"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>142</v>
+      </c>
+      <c r="B146" s="22"/>
+      <c r="C146" s="23"/>
+      <c r="D146" s="22"/>
+      <c r="E146" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="F146" s="22"/>
+      <c r="G146" s="23"/>
+      <c r="H146" s="22"/>
+      <c r="I146" s="23"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>143</v>
+      </c>
+      <c r="B147" s="22"/>
+      <c r="C147" s="23"/>
+      <c r="D147" s="22"/>
+      <c r="E147" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="F147" s="22"/>
+      <c r="G147" s="23"/>
+      <c r="H147" s="22"/>
+      <c r="I147" s="23"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>144</v>
+      </c>
+      <c r="B148" s="22"/>
+      <c r="C148" s="23"/>
+      <c r="D148" s="22"/>
+      <c r="E148" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="F148" s="22"/>
+      <c r="G148" s="23"/>
+      <c r="H148" s="22"/>
+      <c r="I148" s="23"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>145</v>
+      </c>
+      <c r="B149" s="22"/>
+      <c r="C149" s="23"/>
+      <c r="D149" s="22"/>
+      <c r="E149" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="F149" s="22"/>
+      <c r="G149" s="23"/>
+      <c r="H149" s="22"/>
+      <c r="I149" s="23"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>146</v>
+      </c>
+      <c r="B150" s="22"/>
+      <c r="C150" s="23"/>
+      <c r="D150" s="22"/>
+      <c r="E150" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="F150" s="22"/>
+      <c r="G150" s="23"/>
+      <c r="H150" s="22"/>
+      <c r="I150" s="23"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>147</v>
+      </c>
+      <c r="B151" s="22"/>
+      <c r="C151" s="23"/>
+      <c r="D151" s="22"/>
+      <c r="E151" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="F151" s="22"/>
+      <c r="G151" s="23"/>
+      <c r="H151" s="22"/>
+      <c r="I151" s="23"/>
+    </row>
+    <row r="152" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>148</v>
+      </c>
+      <c r="B152" s="22"/>
+      <c r="C152" s="23"/>
+      <c r="D152" s="22"/>
+      <c r="E152" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="F152" s="22"/>
+      <c r="G152" s="23"/>
+      <c r="H152" s="22"/>
+      <c r="I152" s="23"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>149</v>
+      </c>
+      <c r="B153" s="22"/>
+      <c r="C153" s="23"/>
+      <c r="D153" s="22"/>
+      <c r="E153" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="F153" s="22"/>
+      <c r="G153" s="23"/>
+      <c r="H153" s="22"/>
+      <c r="I153" s="23"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>150</v>
+      </c>
+      <c r="B154" s="22"/>
+      <c r="C154" s="23"/>
+      <c r="D154" s="22"/>
+      <c r="E154" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="F154" s="22"/>
+      <c r="G154" s="23"/>
+      <c r="H154" s="22"/>
+      <c r="I154" s="23"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>151</v>
+      </c>
+      <c r="B155" s="22"/>
+      <c r="C155" s="23"/>
+      <c r="D155" s="22"/>
+      <c r="E155" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="F155" s="22"/>
+      <c r="G155" s="23"/>
+      <c r="H155" s="22"/>
+      <c r="I155" s="23"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>152</v>
+      </c>
+      <c r="B156" s="22"/>
+      <c r="C156" s="23"/>
+      <c r="D156" s="22"/>
+      <c r="E156" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="F156" s="22"/>
+      <c r="G156" s="23"/>
+      <c r="H156" s="22"/>
+      <c r="I156" s="23"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>153</v>
+      </c>
+      <c r="B157" s="22"/>
+      <c r="C157" s="23"/>
+      <c r="D157" s="22"/>
+      <c r="E157" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="F157" s="22"/>
+      <c r="G157" s="23"/>
+      <c r="H157" s="22"/>
+      <c r="I157" s="23"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>154</v>
+      </c>
+      <c r="B158" s="22"/>
+      <c r="C158" s="23"/>
+      <c r="D158" s="22"/>
+      <c r="E158" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="F158" s="22"/>
+      <c r="G158" s="23"/>
+      <c r="H158" s="22"/>
+      <c r="I158" s="23"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>155</v>
+      </c>
+      <c r="B159" s="22"/>
+      <c r="C159" s="23"/>
+      <c r="D159" s="22"/>
+      <c r="E159" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="F159" s="22"/>
+      <c r="G159" s="23"/>
+      <c r="H159" s="22"/>
+      <c r="I159" s="23"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>156</v>
+      </c>
+      <c r="B160" s="22"/>
+      <c r="C160" s="23"/>
+      <c r="D160" s="22"/>
+      <c r="E160" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="F160" s="22"/>
+      <c r="G160" s="23"/>
+      <c r="H160" s="22"/>
+      <c r="I160" s="23"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>157</v>
+      </c>
+      <c r="B161" s="22"/>
+      <c r="C161" s="23"/>
+      <c r="D161" s="22"/>
+      <c r="E161" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="F161" s="22"/>
+      <c r="G161" s="23"/>
+      <c r="H161" s="22"/>
+      <c r="I161" s="23"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>158</v>
+      </c>
+      <c r="B162" s="22"/>
+      <c r="C162" s="23"/>
+      <c r="D162" s="22"/>
+      <c r="E162" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="F162" s="22"/>
+      <c r="G162" s="23"/>
+      <c r="H162" s="22"/>
+      <c r="I162" s="23"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>159</v>
+      </c>
+      <c r="B163" s="22"/>
+      <c r="C163" s="23"/>
+      <c r="D163" s="22"/>
+      <c r="E163" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F163" s="22"/>
+      <c r="G163" s="23"/>
+      <c r="H163" s="22"/>
+      <c r="I163" s="23"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>160</v>
+      </c>
+      <c r="B164" s="20"/>
+      <c r="C164" s="21"/>
+      <c r="D164" s="20"/>
+      <c r="E164" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="F164" s="20"/>
+      <c r="G164" s="21"/>
+      <c r="H164" s="20"/>
+      <c r="I164" s="21"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>161</v>
+      </c>
+      <c r="B165" s="20"/>
+      <c r="C165" s="21"/>
+      <c r="D165" s="20"/>
+      <c r="E165" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="F165" s="20"/>
+      <c r="G165" s="21"/>
+      <c r="H165" s="20"/>
+      <c r="I165" s="21"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>162</v>
+      </c>
+      <c r="B166" s="20"/>
+      <c r="C166" s="21"/>
+      <c r="D166" s="20"/>
+      <c r="E166" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="F166" s="20"/>
+      <c r="G166" s="21"/>
+      <c r="H166" s="20"/>
+      <c r="I166" s="21"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>163</v>
+      </c>
+      <c r="B167" s="20"/>
+      <c r="C167" s="21"/>
+      <c r="D167" s="20"/>
+      <c r="E167" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="F167" s="20"/>
+      <c r="G167" s="21"/>
+      <c r="H167" s="20"/>
+      <c r="I167" s="21"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>164</v>
+      </c>
+      <c r="B168" s="20"/>
+      <c r="C168" s="21"/>
+      <c r="D168" s="20"/>
+      <c r="E168" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="F168" s="20"/>
+      <c r="G168" s="21"/>
+      <c r="H168" s="20"/>
+      <c r="I168" s="21"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>165</v>
+      </c>
+      <c r="B169" s="20"/>
+      <c r="C169" s="21"/>
+      <c r="D169" s="20"/>
+      <c r="E169" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="F169" s="20"/>
+      <c r="G169" s="21"/>
+      <c r="H169" s="20"/>
+      <c r="I169" s="21"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>166</v>
+      </c>
+      <c r="B170" s="20"/>
+      <c r="C170" s="21"/>
+      <c r="D170" s="20"/>
+      <c r="E170" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="F170" s="20"/>
+      <c r="G170" s="21"/>
+      <c r="H170" s="20"/>
+      <c r="I170" s="21"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>167</v>
+      </c>
+      <c r="B171" s="20"/>
+      <c r="C171" s="21"/>
+      <c r="D171" s="20"/>
+      <c r="E171" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="F171" s="20"/>
+      <c r="G171" s="21"/>
+      <c r="H171" s="20"/>
+      <c r="I171" s="21"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>168</v>
+      </c>
+      <c r="B172" s="20"/>
+      <c r="C172" s="21"/>
+      <c r="D172" s="20"/>
+      <c r="E172" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="F172" s="20"/>
+      <c r="G172" s="21"/>
+      <c r="H172" s="20"/>
+      <c r="I172" s="21"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>169</v>
+      </c>
+      <c r="B173" s="20"/>
+      <c r="C173" s="21"/>
+      <c r="D173" s="20"/>
+      <c r="E173" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="F173" s="20"/>
+      <c r="G173" s="21"/>
+      <c r="H173" s="20"/>
+      <c r="I173" s="21"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>170</v>
+      </c>
+      <c r="B174" s="20"/>
+      <c r="C174" s="21"/>
+      <c r="D174" s="20"/>
+      <c r="E174" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="F174" s="20"/>
+      <c r="G174" s="21"/>
+      <c r="H174" s="20"/>
+      <c r="I174" s="21"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>171</v>
+      </c>
+      <c r="B175" s="20"/>
+      <c r="C175" s="21"/>
+      <c r="D175" s="20"/>
+      <c r="E175" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="F175" s="20"/>
+      <c r="G175" s="21"/>
+      <c r="H175" s="20"/>
+      <c r="I175" s="21"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>172</v>
+      </c>
+      <c r="B176" s="20"/>
+      <c r="C176" s="21"/>
+      <c r="D176" s="20"/>
+      <c r="E176" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="F176" s="20"/>
+      <c r="G176" s="21"/>
+      <c r="H176" s="20"/>
+      <c r="I176" s="21"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>173</v>
+      </c>
+      <c r="B177" s="20"/>
+      <c r="C177" s="21"/>
+      <c r="D177" s="20"/>
+      <c r="E177" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F177" s="20"/>
+      <c r="G177" s="21"/>
+      <c r="H177" s="20"/>
+      <c r="I177" s="21"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>174</v>
+      </c>
+      <c r="B178" s="20"/>
+      <c r="C178" s="21"/>
+      <c r="D178" s="20"/>
+      <c r="E178" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="F178" s="20"/>
+      <c r="G178" s="21"/>
+      <c r="H178" s="20"/>
+      <c r="I178" s="21"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>175</v>
+      </c>
+      <c r="B179" s="20"/>
+      <c r="C179" s="21"/>
+      <c r="D179" s="20"/>
+      <c r="E179" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="F179" s="20"/>
+      <c r="G179" s="21"/>
+      <c r="H179" s="20"/>
+      <c r="I179" s="21"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>176</v>
+      </c>
+      <c r="B180" s="20"/>
+      <c r="C180" s="21"/>
+      <c r="D180" s="20"/>
+      <c r="E180" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="F180" s="20"/>
+      <c r="G180" s="21"/>
+      <c r="H180" s="20"/>
+      <c r="I180" s="21"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>177</v>
+      </c>
+      <c r="B181" s="20"/>
+      <c r="C181" s="21"/>
+      <c r="D181" s="20"/>
+      <c r="E181" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="F181" s="20"/>
+      <c r="G181" s="21"/>
+      <c r="H181" s="20"/>
+      <c r="I181" s="21"/>
+    </row>
+    <row r="182" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>178</v>
+      </c>
+      <c r="B182" s="20"/>
+      <c r="C182" s="21"/>
+      <c r="D182" s="20"/>
+      <c r="E182" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="F182" s="20"/>
+      <c r="G182" s="21"/>
+      <c r="H182" s="20"/>
+      <c r="I182" s="21"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>179</v>
+      </c>
+      <c r="B183" s="20"/>
+      <c r="C183" s="21"/>
+      <c r="D183" s="20"/>
+      <c r="E183" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="F183" s="20"/>
+      <c r="G183" s="21"/>
+      <c r="H183" s="20"/>
+      <c r="I183" s="21"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>180</v>
+      </c>
+      <c r="B184" s="8"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="8"/>
+      <c r="E184" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="F184" s="8"/>
+      <c r="G184" s="9"/>
+      <c r="H184" s="8"/>
+      <c r="I184" s="9"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>181</v>
+      </c>
+      <c r="B185" s="8"/>
+      <c r="C185" s="9"/>
+      <c r="D185" s="8"/>
+      <c r="E185" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="F185" s="8"/>
+      <c r="G185" s="9"/>
+      <c r="H185" s="8"/>
+      <c r="I185" s="9"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>182</v>
+      </c>
+      <c r="B186" s="8"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="8"/>
+      <c r="E186" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F186" s="8"/>
+      <c r="G186" s="9"/>
+      <c r="H186" s="8"/>
+      <c r="I186" s="9"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>183</v>
+      </c>
+      <c r="B187" s="8"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="8"/>
+      <c r="E187" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="F187" s="8"/>
+      <c r="G187" s="9"/>
+      <c r="H187" s="8"/>
+      <c r="I187" s="9"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>184</v>
+      </c>
+      <c r="B188" s="8"/>
+      <c r="C188" s="9"/>
+      <c r="D188" s="8"/>
+      <c r="E188" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="F188" s="8"/>
+      <c r="G188" s="9"/>
+      <c r="H188" s="8"/>
+      <c r="I188" s="9"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>185</v>
+      </c>
+      <c r="B189" s="8"/>
+      <c r="C189" s="9"/>
+      <c r="D189" s="8"/>
+      <c r="E189" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F189" s="8"/>
+      <c r="G189" s="9"/>
+      <c r="H189" s="8"/>
+      <c r="I189" s="9"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>186</v>
+      </c>
+      <c r="B190" s="8"/>
+      <c r="C190" s="9"/>
+      <c r="D190" s="8"/>
+      <c r="E190" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="F190" s="8"/>
+      <c r="G190" s="9"/>
+      <c r="H190" s="8"/>
+      <c r="I190" s="9"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>187</v>
+      </c>
+      <c r="B191" s="8"/>
+      <c r="C191" s="9"/>
+      <c r="D191" s="8"/>
+      <c r="E191" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="F191" s="8"/>
+      <c r="G191" s="9"/>
+      <c r="H191" s="8"/>
+      <c r="I191" s="9"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>188</v>
+      </c>
+      <c r="B192" s="8"/>
+      <c r="C192" s="9"/>
+      <c r="D192" s="8"/>
+      <c r="E192" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="F192" s="8"/>
+      <c r="G192" s="9"/>
+      <c r="H192" s="8"/>
+      <c r="I192" s="9"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>189</v>
+      </c>
+      <c r="B193" s="8"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="8"/>
+      <c r="E193" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F193" s="8"/>
+      <c r="G193" s="9"/>
+      <c r="H193" s="8"/>
+      <c r="I193" s="9"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>190</v>
+      </c>
+      <c r="B194" s="8"/>
+      <c r="C194" s="9"/>
+      <c r="D194" s="8"/>
+      <c r="E194" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="F194" s="8"/>
+      <c r="G194" s="9"/>
+      <c r="H194" s="8"/>
+      <c r="I194" s="9"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>191</v>
+      </c>
+      <c r="B195" s="8"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="8"/>
+      <c r="E195" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="F195" s="8"/>
+      <c r="G195" s="9"/>
+      <c r="H195" s="8"/>
+      <c r="I195" s="9"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>192</v>
+      </c>
+      <c r="B196" s="8"/>
+      <c r="C196" s="9"/>
+      <c r="D196" s="8"/>
+      <c r="E196" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F196" s="8"/>
+      <c r="G196" s="9"/>
+      <c r="H196" s="8"/>
+      <c r="I196" s="9"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>193</v>
+      </c>
+      <c r="B197" s="8"/>
+      <c r="C197" s="9"/>
+      <c r="D197" s="8"/>
+      <c r="E197" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="F197" s="8"/>
+      <c r="G197" s="9"/>
+      <c r="H197" s="8"/>
+      <c r="I197" s="9"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>194</v>
+      </c>
+      <c r="B198" s="8"/>
+      <c r="C198" s="9"/>
+      <c r="D198" s="8"/>
+      <c r="E198" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="F198" s="8"/>
+      <c r="G198" s="9"/>
+      <c r="H198" s="8"/>
+      <c r="I198" s="9"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>195</v>
+      </c>
+      <c r="B199" s="8"/>
+      <c r="C199" s="9"/>
+      <c r="D199" s="8"/>
+      <c r="E199" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="F199" s="8"/>
+      <c r="G199" s="9"/>
+      <c r="H199" s="8"/>
+      <c r="I199" s="9"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>196</v>
+      </c>
+      <c r="B200" s="8"/>
+      <c r="C200" s="9"/>
+      <c r="D200" s="8"/>
+      <c r="E200" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="F200" s="8"/>
+      <c r="G200" s="9"/>
+      <c r="H200" s="8"/>
+      <c r="I200" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>